<commit_message>
documentation and minor edits for R0 fit
</commit_message>
<xml_diff>
--- a/param-model/_all_param_value_source.xlsx
+++ b/param-model/_all_param_value_source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-440" windowWidth="28820" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-440" windowWidth="28020" windowHeight="28460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -804,17 +804,7 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1165,8 +1155,8 @@
   <dimension ref="B1:H63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1848,7 +1838,7 @@
         <v>75</v>
       </c>
       <c r="E33" s="4">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="6" t="s">
@@ -1886,7 +1876,7 @@
         <v>79</v>
       </c>
       <c r="E35" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="6" t="s">
@@ -1962,7 +1952,7 @@
         <v>88</v>
       </c>
       <c r="E39" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="6" t="s">
@@ -2144,12 +2134,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G57">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>G2="Arbitrary"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G13">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>G12="Arbitrary"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add more studies for parameter comparison
</commit_message>
<xml_diff>
--- a/param-model/_all_param_value_source.xlsx
+++ b/param-model/_all_param_value_source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15600" yWindow="3500" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="196">
   <si>
     <t>PARAMETER</t>
   </si>
@@ -627,6 +627,33 @@
   </si>
   <si>
     <t>Manitoba</t>
+  </si>
+  <si>
+    <t>Araz 2012</t>
+  </si>
+  <si>
+    <t>Arizona, USA</t>
+  </si>
+  <si>
+    <t>ODE</t>
+  </si>
+  <si>
+    <t>Lee 2010</t>
+  </si>
+  <si>
+    <t>Washington DC, USA</t>
+  </si>
+  <si>
+    <t>Wood 2009</t>
+  </si>
+  <si>
+    <t>theoretical</t>
+  </si>
+  <si>
+    <t>Mylius 2008</t>
+  </si>
+  <si>
+    <t>The Netherlands</t>
   </si>
 </sst>
 </file>
@@ -763,8 +790,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -971,7 +1000,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="133">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1037,6 +1066,7 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1102,6 +1132,7 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1298,7 +1329,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="H8:L17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -2710,13 +2741,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2728,7 +2759,7 @@
     <col min="8" max="8" width="11" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="7.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.83203125" style="18" customWidth="1"/>
     <col min="14" max="15" width="15" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5" style="18" bestFit="1" customWidth="1"/>
@@ -3219,6 +3250,155 @@
         <v>0.3</v>
       </c>
       <c r="Y8" s="26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="18">
+        <v>4</v>
+      </c>
+      <c r="E9" s="18">
+        <v>6</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1.4</v>
+      </c>
+      <c r="G9" s="18">
+        <v>1.4</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="M9" s="18">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="P9" s="18">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2</v>
+      </c>
+      <c r="F11" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="G11" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="P11" s="18">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>180</v>
+      </c>
+      <c r="R11" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="S11" s="18">
+        <v>1</v>
+      </c>
+      <c r="X11" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="18">
+        <v>1.95</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1.73</v>
+      </c>
+      <c r="G12" s="18">
+        <v>1.73</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="P12" s="18">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>86</v>
+      </c>
+      <c r="R12" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="S12" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="X12" s="18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Y12" s="18">
         <v>0.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
R script to check all fits
</commit_message>
<xml_diff>
--- a/param-model/_all_param_value_source.xlsx
+++ b/param-model/_all_param_value_source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="3500" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2900" yWindow="0" windowWidth="32800" windowHeight="27980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="196">
   <si>
     <t>PARAMETER</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>Mean of contact rate distribution</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>contact_rate_stddev</t>
@@ -654,6 +651,9 @@
   </si>
   <si>
     <t>The Netherlands</t>
+  </si>
+  <si>
+    <t>number of contacts per capita per day</t>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,12 +760,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,7 +784,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -924,8 +918,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -972,9 +970,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1000,7 +995,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1067,6 +1062,8 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1133,6 +1130,8 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1329,7 +1328,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="H8:L17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -1740,9 +1739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H63"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1752,7 +1751,7 @@
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="31.1640625" style="10" customWidth="1"/>
   </cols>
@@ -1816,10 +1815,10 @@
         <v>9</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="66">
@@ -1839,7 +1838,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H4" s="12"/>
     </row>
@@ -1860,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="66">
@@ -1883,7 +1882,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H6" s="12"/>
     </row>
@@ -1961,10 +1960,10 @@
         <v>9</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="22">
@@ -1984,7 +1983,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="13"/>
     </row>
@@ -1993,17 +1992,17 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -2012,20 +2011,20 @@
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="66">
@@ -2033,20 +2032,20 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="4">
         <v>0.1</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="22">
@@ -2164,7 +2163,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" s="4">
         <v>0.43</v>
@@ -2211,7 +2210,7 @@
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H22" s="13"/>
     </row>
@@ -2270,7 +2269,7 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H25" s="13"/>
     </row>
@@ -2314,9 +2313,9 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" ht="45">
       <c r="B28" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>62</v>
@@ -2327,82 +2326,80 @@
       <c r="E28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>64</v>
+      <c r="F28" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="F29" s="4"/>
       <c r="G29" s="6"/>
       <c r="H29" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="77">
       <c r="B30" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E30" s="4">
         <v>15</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="2:8" ht="66">
       <c r="B31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="E31" s="4">
         <v>3</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="2:8" ht="30">
       <c r="B32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="E32" s="4">
         <v>1</v>
@@ -2415,13 +2412,13 @@
     </row>
     <row r="33" spans="2:8" ht="30">
       <c r="B33" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
@@ -2434,13 +2431,13 @@
     </row>
     <row r="34" spans="2:8" ht="30">
       <c r="B34" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="E34" s="4">
         <v>1</v>
@@ -2453,13 +2450,13 @@
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="E35" s="4">
         <v>1</v>
@@ -2472,13 +2469,13 @@
     </row>
     <row r="36" spans="2:8" ht="45">
       <c r="B36" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="E36" s="4">
         <v>0.1</v>
@@ -2491,13 +2488,13 @@
     </row>
     <row r="37" spans="2:8" ht="30">
       <c r="B37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E37" s="4">
         <v>0.98</v>
@@ -2510,13 +2507,13 @@
     </row>
     <row r="38" spans="2:8" ht="30">
       <c r="B38" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="E38" s="4">
         <v>0.4</v>
@@ -2529,13 +2526,13 @@
     </row>
     <row r="39" spans="2:8" ht="30">
       <c r="B39" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E39" s="4">
         <v>0.2</v>
@@ -2548,13 +2545,13 @@
     </row>
     <row r="40" spans="2:8" ht="45">
       <c r="B40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
@@ -2563,19 +2560,19 @@
         <v>9</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="2:8" ht="45">
       <c r="B41" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="E41" s="4">
         <v>0.1</v>
@@ -2585,82 +2582,82 @@
         <v>23</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="30">
       <c r="B42" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="E42" s="4">
         <v>0.1</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="2:8" ht="30">
       <c r="B43" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E43" s="4">
         <v>0.1</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="2:8" ht="30">
       <c r="B44" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E44" s="4">
         <v>12</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="2:8" ht="30">
       <c r="B45" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E45" s="4">
         <v>0</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H45" s="13"/>
     </row>
@@ -2743,7 +2740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2754,651 +2751,651 @@
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="6.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="18" customWidth="1"/>
-    <col min="14" max="15" width="15" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" style="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="16.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="6.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="17" customWidth="1"/>
+    <col min="14" max="15" width="15" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="16.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="24" customFormat="1">
-      <c r="A1" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:25" s="23" customFormat="1">
+      <c r="A1" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="Q1" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="R1" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="W1" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="X1" s="25" t="s">
+      <c r="X1" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y1" s="24" t="s">
         <v>173</v>
-      </c>
-      <c r="Y1" s="25" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
         <v>168</v>
       </c>
-      <c r="B2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
         <v>170</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>3.5</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="25">
         <v>2.5</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>1.3</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>1.3</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="25">
         <v>0.15</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="25">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="25">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="25">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="25">
         <v>0</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="25">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26">
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25">
         <v>225</v>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3" s="25">
         <v>225</v>
       </c>
-      <c r="R3" s="26">
+      <c r="R3" s="25">
         <v>0.3</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="25">
         <v>0.75</v>
       </c>
-      <c r="T3" s="26">
+      <c r="T3" s="25">
         <v>0.6</v>
       </c>
-      <c r="U3" s="26">
+      <c r="U3" s="25">
         <v>0.6</v>
       </c>
-      <c r="V3" s="26">
+      <c r="V3" s="25">
         <v>1</v>
       </c>
-      <c r="W3" s="26">
+      <c r="W3" s="25">
         <v>1</v>
       </c>
-      <c r="X3" s="26">
+      <c r="X3" s="25">
         <v>0.7</v>
       </c>
-      <c r="Y3" s="26">
+      <c r="Y3" s="25">
         <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
         <v>175</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25">
         <v>4</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>1.2</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <v>1.8</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25">
         <v>5</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="25">
         <v>90</v>
       </c>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26">
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25">
         <v>0.67</v>
       </c>
-      <c r="U4" s="26">
+      <c r="U4" s="25">
         <v>0.67</v>
       </c>
-      <c r="V4" s="26">
+      <c r="V4" s="25">
         <v>0.5</v>
       </c>
-      <c r="W4" s="26">
+      <c r="W4" s="25">
         <v>0.5</v>
       </c>
-      <c r="X4" s="26">
+      <c r="X4" s="25">
         <v>0.1</v>
       </c>
-      <c r="Y4" s="26">
+      <c r="Y4" s="25">
         <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" t="s">
         <v>180</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>1.9</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>6</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>1.4</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>2.4</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26">
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25">
         <v>-1</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="25">
         <v>10</v>
       </c>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26">
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25">
         <v>0.67</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="25">
         <v>0.67</v>
       </c>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D6" s="26">
+        <v>170</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="25">
         <v>2.7</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>3.25</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>1.3</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>2</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <v>0.2</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>0.5</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26">
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="25">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="25">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="25">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="25">
         <v>28</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="25">
         <v>84</v>
       </c>
-      <c r="R6" s="26">
+      <c r="R6" s="25">
         <v>0.25</v>
       </c>
-      <c r="S6" s="26">
+      <c r="S6" s="25">
         <v>0.75</v>
       </c>
-      <c r="T6" s="26">
+      <c r="T6" s="25">
         <v>0.6</v>
       </c>
-      <c r="U6" s="26">
+      <c r="U6" s="25">
         <v>0.6</v>
       </c>
-      <c r="V6" s="26">
+      <c r="V6" s="25">
         <v>1</v>
       </c>
-      <c r="W6" s="26">
+      <c r="W6" s="25">
         <v>1</v>
       </c>
-      <c r="X6" s="26">
+      <c r="X6" s="25">
         <v>0.3</v>
       </c>
-      <c r="Y6" s="26">
+      <c r="Y6" s="25">
         <v>0.7</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25">
         <v>0.2</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>0.3</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="25">
         <v>0.04</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="25">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="25">
         <v>5.3E-3</v>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="25">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O7" s="26">
+      <c r="O7" s="25">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="25">
         <v>-112</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="25">
         <v>112</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="25">
         <v>0.8</v>
       </c>
-      <c r="S7" s="26">
+      <c r="S7" s="25">
         <v>0.8</v>
       </c>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26">
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25">
         <v>0.4</v>
       </c>
-      <c r="Y7" s="26">
+      <c r="Y7" s="25">
         <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" t="s">
         <v>185</v>
       </c>
-      <c r="B8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="26">
+      <c r="C8" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="25">
         <v>1.5</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="25">
         <v>3.38</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="25">
         <v>1.3</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="25">
         <v>2</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26">
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="25">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="25">
         <v>-14</v>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="25">
         <v>28</v>
       </c>
-      <c r="R8" s="26">
+      <c r="R8" s="25">
         <v>0</v>
       </c>
-      <c r="S8" s="26">
+      <c r="S8" s="25">
         <v>0.5</v>
       </c>
-      <c r="T8" s="26">
+      <c r="T8" s="25">
         <v>0.6</v>
       </c>
-      <c r="U8" s="26">
+      <c r="U8" s="25">
         <v>0.6</v>
       </c>
-      <c r="V8" s="26">
+      <c r="V8" s="25">
         <v>0.5</v>
       </c>
-      <c r="W8" s="26">
+      <c r="W8" s="25">
         <v>0.5</v>
       </c>
-      <c r="X8" s="26">
+      <c r="X8" s="25">
         <v>0.3</v>
       </c>
-      <c r="Y8" s="26">
+      <c r="Y8" s="25">
         <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" t="s">
         <v>187</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>4</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>6</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>1.4</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <v>1.4</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>0.3</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="17">
         <v>1E-4</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="17">
         <v>100</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="Q9" s="17">
         <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" t="s">
         <v>190</v>
       </c>
-      <c r="B10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" s="18">
+      <c r="C10" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="17">
         <v>0.33500000000000002</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="17">
         <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" t="s">
         <v>192</v>
       </c>
-      <c r="B11" t="s">
-        <v>193</v>
-      </c>
       <c r="C11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="18">
+        <v>171</v>
+      </c>
+      <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>2</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>1.5</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>2.5</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>0</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="17">
         <v>0.7</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="17">
         <v>60</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="17">
         <v>180</v>
       </c>
-      <c r="R11" s="18">
+      <c r="R11" s="17">
         <v>0.5</v>
       </c>
-      <c r="S11" s="18">
+      <c r="S11" s="17">
         <v>1</v>
       </c>
-      <c r="X11" s="18">
+      <c r="X11" s="17">
         <v>0</v>
       </c>
-      <c r="Y11" s="18">
+      <c r="Y11" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" t="s">
         <v>194</v>
       </c>
-      <c r="B12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D12" s="18">
+      <c r="C12" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="17">
         <v>1.95</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>1.6</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>1.73</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>1.73</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>0.6</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="17">
         <v>0.8</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="17">
         <v>36</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="Q12" s="17">
         <v>86</v>
       </c>
-      <c r="R12" s="18">
+      <c r="R12" s="17">
         <v>0.35</v>
       </c>
-      <c r="S12" s="18">
+      <c r="S12" s="17">
         <v>0.35</v>
       </c>
-      <c r="X12" s="18">
+      <c r="X12" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="Y12" s="18">
+      <c r="Y12" s="17">
         <v>0.8</v>
       </c>
     </row>
@@ -3426,7 +3423,7 @@
   <cols>
     <col min="1" max="1" width="14.5" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="20"/>
+    <col min="3" max="4" width="10.83203125" style="19"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="7" width="1.6640625" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -3436,358 +3433,358 @@
     <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="18" customFormat="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:12" s="17" customFormat="1">
+      <c r="A1" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="21">
+        <v>135</v>
+      </c>
+      <c r="C2" s="20">
         <v>0.2</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="21">
+        <v>124</v>
+      </c>
+      <c r="C3" s="20">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="21">
+        <v>125</v>
+      </c>
+      <c r="C4" s="20">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>5.3E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="21">
+        <v>126</v>
+      </c>
+      <c r="C5" s="20">
         <v>0.8</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="21">
+        <v>133</v>
+      </c>
+      <c r="C6" s="20">
         <v>10</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="21">
+        <v>127</v>
+      </c>
+      <c r="C7" s="20">
         <v>0.43</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>0.8</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>137</v>
+      <c r="E7" s="18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="20">
+        <v>132</v>
+      </c>
+      <c r="C8" s="19">
         <v>-112</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>112</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>142</v>
+      <c r="I8" s="21" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>0.2</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>0.5</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="21">
+        <v>124</v>
+      </c>
+      <c r="C10" s="20">
         <v>0.01</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>0.01</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" t="s">
         <v>143</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>144</v>
       </c>
-      <c r="J10" t="s">
-        <v>145</v>
-      </c>
       <c r="K10" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" t="s">
         <v>144</v>
-      </c>
-      <c r="L10" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="21">
+        <v>125</v>
+      </c>
+      <c r="C11" s="20">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" s="23">
+      <c r="H11" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" s="22">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="22">
         <v>5.3E-3</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="22">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="22">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.26</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="21">
-        <v>0.26</v>
-      </c>
-      <c r="D12" s="21">
-        <v>0.75</v>
-      </c>
-      <c r="E12" t="s">
-        <v>139</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <v>0.2</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="22">
         <v>0.3</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="22">
         <v>0.2</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="22">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="21">
+        <v>133</v>
+      </c>
+      <c r="C13" s="20">
         <v>0.15</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>3.75</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="23">
+      <c r="H13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="22">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="22">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="22">
         <v>0.01</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="22">
         <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="21">
+        <v>127</v>
+      </c>
+      <c r="C14" s="20">
         <v>0.3</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>0.7</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="I14" s="23">
+      <c r="E14" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="I14" s="22">
         <v>10</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="22">
         <v>30</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="22">
         <v>0.15</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="22">
         <v>3.75</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="20">
+        <v>132</v>
+      </c>
+      <c r="C15" s="19">
         <v>30</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>90</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="J15" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="K15" s="22">
+        <v>0.26</v>
+      </c>
+      <c r="L15" s="22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="H16" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I16" s="22">
+        <v>0.43</v>
+      </c>
+      <c r="J16" s="22">
         <v>0.8</v>
       </c>
-      <c r="J15" s="23">
-        <v>0.8</v>
-      </c>
-      <c r="K15" s="23">
-        <v>0.26</v>
-      </c>
-      <c r="L15" s="23">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="H16" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I16" s="23">
-        <v>0.43</v>
-      </c>
-      <c r="J16" s="23">
-        <v>0.8</v>
-      </c>
-      <c r="K16" s="23">
+      <c r="K16" s="22">
         <v>0.3</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="22">
         <v>0.7</v>
       </c>
     </row>
     <row r="17" spans="8:12">
-      <c r="H17" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" s="23">
+      <c r="H17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="22">
         <v>-112</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="22">
         <v>112</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="22">
         <v>30</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="22">
         <v>90</v>
       </c>
     </row>

</xml_diff>